<commit_message>
iems data-driven test case 2nd version
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.3.1.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED58C652-ACD0-4629-A669-D92F599FA9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42777DD2-F423-40B5-8ED0-84F0D5BAC97B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="113">
   <si>
     <t>name</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>iems-connector-test-8-var2</t>
-  </si>
-  <si>
-    <t>run_time</t>
   </si>
   <si>
     <t>iems-connector-test-8-var3</t>
@@ -727,8 +724,8 @@
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H55" sqref="H55"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1477,7 +1474,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3">
@@ -1490,7 +1487,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1502,7 +1499,7 @@
         <v>14</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3">
@@ -1515,7 +1512,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>5</v>
@@ -1527,7 +1524,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3">
@@ -1540,7 +1537,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
@@ -1552,7 +1549,7 @@
         <v>14</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3">
@@ -1565,7 +1562,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -1577,7 +1574,7 @@
         <v>16</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3">
@@ -1590,7 +1587,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>5</v>
@@ -1602,7 +1599,7 @@
         <v>14</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3">
@@ -1615,7 +1612,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
@@ -1627,7 +1624,7 @@
         <v>16</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
@@ -1640,7 +1637,7 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>5</v>
@@ -1652,7 +1649,7 @@
         <v>14</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3">
@@ -1665,7 +1662,7 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>5</v>
@@ -1677,7 +1674,7 @@
         <v>16</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3">
@@ -1690,10 +1687,10 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1712,15 +1709,15 @@
         <v>106601</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1739,15 +1736,15 @@
         <v>106601</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1766,15 +1763,15 @@
         <v>106601</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1793,12 +1790,12 @@
         <v>106601</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
@@ -1823,7 +1820,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>5</v>
@@ -1846,7 +1843,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -1871,7 +1868,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
@@ -1894,7 +1891,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>5</v>
@@ -1921,7 +1918,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>5</v>
@@ -1946,7 +1943,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>5</v>
@@ -1973,7 +1970,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>5</v>
@@ -1998,7 +1995,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>5</v>
@@ -2025,7 +2022,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>5</v>
@@ -2050,7 +2047,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>5</v>
@@ -2077,7 +2074,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>5</v>
@@ -2102,7 +2099,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>5</v>
@@ -2127,7 +2124,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>5</v>
@@ -2150,7 +2147,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>5</v>
@@ -2175,7 +2172,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>5</v>
@@ -2198,7 +2195,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>5</v>
@@ -2223,7 +2220,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>5</v>
@@ -2246,7 +2243,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>5</v>
@@ -2271,7 +2268,7 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
remove iems-connector-test-5-var1/2 (domain name is not present)
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42777DD2-F423-40B5-8ED0-84F0D5BAC97B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88487C1C-B0E4-403F-AE5F-A65FEA216DED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="110">
   <si>
     <t>name</t>
   </si>
@@ -172,15 +172,6 @@
   </si>
   <si>
     <t>iEMS</t>
-  </si>
-  <si>
-    <t>iems-connector-test-5-var1</t>
-  </si>
-  <si>
-    <t>iems-connector-test-5-var2</t>
-  </si>
-  <si>
-    <t>bad request (domain name is not present)</t>
   </si>
   <si>
     <t>iems-connector-test-6-var1</t>
@@ -721,11 +712,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G27" sqref="G27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -1162,15 +1153,17 @@
         <v>49</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="4">
-        <v>12321321</v>
-      </c>
-      <c r="E18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="F18" s="3" t="s">
         <v>14</v>
       </c>
@@ -1179,25 +1172,25 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
-      <c r="L18" s="3">
-        <v>106602</v>
-      </c>
+      <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="4">
-        <v>12321321</v>
-      </c>
-      <c r="E19" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="F19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1206,14 +1199,12 @@
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3">
-        <v>106602</v>
-      </c>
+      <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>5</v>
@@ -1225,7 +1216,7 @@
         <v>48</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>14</v>
@@ -1240,19 +1231,19 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>16</v>
@@ -1267,7 +1258,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
@@ -1279,7 +1270,7 @@
         <v>48</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>14</v>
@@ -1294,19 +1285,19 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>16</v>
@@ -1321,10 +1312,10 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>21</v>
@@ -1332,8 +1323,8 @@
       <c r="D24" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>61</v>
+      <c r="E24" s="4">
+        <v>321321</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>14</v>
@@ -1343,15 +1334,19 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
+      <c r="L24" s="3">
+        <v>106107</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>5</v>
+        <v>63</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>32</v>
@@ -1359,8 +1354,8 @@
       <c r="D25" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>61</v>
+      <c r="E25" s="4">
+        <v>321321</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>16</v>
@@ -1370,74 +1365,66 @@
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="L25" s="3">
+        <v>106107</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="4">
-        <v>321321</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="3"/>
+      <c r="G26" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="I26" s="3">
+        <v>10</v>
+      </c>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
-      <c r="L26" s="3">
-        <v>106107</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E27" s="4">
-        <v>321321</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="I27" s="3">
+        <v>10</v>
+      </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-      <c r="L27" s="3">
-        <v>106107</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>67</v>
-      </c>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1448,8 +1435,8 @@
       <c r="F28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G28" s="3" t="s">
-        <v>30</v>
+      <c r="G28" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3">
@@ -1462,7 +1449,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
@@ -1473,8 +1460,8 @@
       <c r="F29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>31</v>
+      <c r="G29" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3">
@@ -1487,7 +1474,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1499,7 +1486,7 @@
         <v>14</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3">
@@ -1512,7 +1499,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>5</v>
@@ -1524,7 +1511,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3">
@@ -1537,7 +1524,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
@@ -1549,7 +1536,7 @@
         <v>14</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3">
@@ -1562,7 +1549,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -1574,7 +1561,7 @@
         <v>16</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3">
@@ -1587,7 +1574,7 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>5</v>
@@ -1599,7 +1586,7 @@
         <v>14</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3">
@@ -1612,7 +1599,7 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>5</v>
@@ -1624,7 +1611,7 @@
         <v>16</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
@@ -1637,10 +1624,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1648,24 +1635,26 @@
       <c r="F36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G36" s="5" t="s">
-        <v>84</v>
+      <c r="G36" s="3">
+        <v>12321</v>
       </c>
       <c r="H36" s="3"/>
-      <c r="I36" s="3">
-        <v>10</v>
-      </c>
+      <c r="I36" s="3"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
+      <c r="L36" s="3">
+        <v>106601</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>5</v>
+        <v>84</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1673,24 +1662,26 @@
       <c r="F37" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>85</v>
+      <c r="G37" s="3">
+        <v>12321</v>
       </c>
       <c r="H37" s="3"/>
-      <c r="I37" s="3">
-        <v>10</v>
-      </c>
+      <c r="I37" s="3"/>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
+      <c r="L37" s="3">
+        <v>106601</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1698,8 +1689,8 @@
       <c r="F38" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G38" s="3">
-        <v>12321</v>
+      <c r="G38" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -1717,7 +1708,7 @@
         <v>88</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1725,8 +1716,8 @@
       <c r="F39" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="3">
-        <v>12321</v>
+      <c r="G39" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -1744,7 +1735,7 @@
         <v>90</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -1753,25 +1744,23 @@
         <v>14</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H40" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="H40" s="3">
+        <v>0</v>
+      </c>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="3">
-        <v>106601</v>
-      </c>
-      <c r="M40" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -1779,23 +1768,19 @@
       <c r="F41" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
       <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
-      <c r="L41" s="3">
-        <v>106601</v>
-      </c>
-      <c r="M41" s="3" t="s">
-        <v>92</v>
-      </c>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
@@ -1809,10 +1794,10 @@
       <c r="G42" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H42" s="3">
+      <c r="H42" s="3"/>
+      <c r="I42" s="3">
         <v>0</v>
       </c>
-      <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
@@ -1820,7 +1805,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>5</v>
@@ -1832,10 +1817,10 @@
         <v>16</v>
       </c>
       <c r="G43" s="3"/>
-      <c r="H43" s="3">
+      <c r="H43" s="3"/>
+      <c r="I43" s="3">
         <v>0</v>
       </c>
-      <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
@@ -1843,7 +1828,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -1857,7 +1842,9 @@
       <c r="G44" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H44" s="3"/>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
       <c r="I44" s="3">
         <v>0</v>
       </c>
@@ -1868,7 +1855,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
@@ -1880,7 +1867,9 @@
         <v>16</v>
       </c>
       <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
       <c r="I45" s="3">
         <v>0</v>
       </c>
@@ -1891,7 +1880,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>5</v>
@@ -1906,10 +1895,10 @@
         <v>30</v>
       </c>
       <c r="H46" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I46" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
@@ -1918,7 +1907,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>5</v>
@@ -1931,10 +1920,10 @@
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I47" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -1943,7 +1932,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>5</v>
@@ -1958,10 +1947,10 @@
         <v>30</v>
       </c>
       <c r="H48" s="3">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="I48" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -1970,7 +1959,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>5</v>
@@ -1983,10 +1972,10 @@
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="I49" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
@@ -1995,7 +1984,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>5</v>
@@ -2010,10 +1999,10 @@
         <v>30</v>
       </c>
       <c r="H50" s="3">
+        <v>2</v>
+      </c>
+      <c r="I50" s="3">
         <v>-2</v>
-      </c>
-      <c r="I50" s="3">
-        <v>10</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
@@ -2022,7 +2011,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>5</v>
@@ -2035,10 +2024,10 @@
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3">
+        <v>2</v>
+      </c>
+      <c r="I51" s="3">
         <v>-2</v>
-      </c>
-      <c r="I51" s="3">
-        <v>10</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2047,7 +2036,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>5</v>
@@ -2064,9 +2053,7 @@
       <c r="H52" s="3">
         <v>2</v>
       </c>
-      <c r="I52" s="3">
-        <v>-2</v>
-      </c>
+      <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
@@ -2074,7 +2061,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>5</v>
@@ -2089,9 +2076,7 @@
       <c r="H53" s="3">
         <v>2</v>
       </c>
-      <c r="I53" s="3">
-        <v>-2</v>
-      </c>
+      <c r="I53" s="3"/>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
       <c r="L53" s="3"/>
@@ -2099,7 +2084,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>5</v>
@@ -2114,7 +2099,7 @@
         <v>30</v>
       </c>
       <c r="H54" s="3">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="I54" s="3"/>
       <c r="J54" s="3"/>
@@ -2124,7 +2109,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>5</v>
@@ -2137,7 +2122,7 @@
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="I55" s="3"/>
       <c r="J55" s="3"/>
@@ -2147,7 +2132,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>5</v>
@@ -2161,10 +2146,10 @@
       <c r="G56" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H56" s="3">
-        <v>-2</v>
-      </c>
-      <c r="I56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3">
+        <v>2</v>
+      </c>
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
@@ -2172,7 +2157,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>5</v>
@@ -2184,10 +2169,10 @@
         <v>16</v>
       </c>
       <c r="G57" s="3"/>
-      <c r="H57" s="3">
-        <v>-2</v>
-      </c>
-      <c r="I57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3">
+        <v>2</v>
+      </c>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
       <c r="L57" s="3"/>
@@ -2195,7 +2180,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>5</v>
@@ -2211,7 +2196,7 @@
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="3">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J58" s="3"/>
       <c r="K58" s="3"/>
@@ -2220,7 +2205,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>5</v>
@@ -2234,60 +2219,12 @@
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="I59" s="3">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3">
-        <v>-2</v>
-      </c>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3">
-        <v>-2</v>
-      </c>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
update motor_current_percent=100.0 on test case
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UserData\workspace-spring-tool-suite-4-4.10.0.RELEASE\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\branches\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4632CA-33E4-410C-954D-EF415C0AF2E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF85E62-B145-4089-B5C6-4C3C36B817A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-14570" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="111">
   <si>
     <t>name</t>
   </si>
@@ -126,9 +126,6 @@
     <t>motor_current_percent=100</t>
   </si>
   <si>
-    <t>motor_current_percent=100 AND condensor_water_inlet_temperature&lt;40.0</t>
-  </si>
-  <si>
     <t>siid&gt;5040 AND siid&lt;10000</t>
   </si>
   <si>
@@ -352,6 +349,18 @@
   </si>
   <si>
     <t>bad request, order input contains invalid field name</t>
+  </si>
+  <si>
+    <t>motor_current_percent=100.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>motor_current_percent=100.0 AND condensor_water_inlet_temperature&lt;40.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>motor_current_percent=100.0</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -362,20 +371,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -713,16 +722,17 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M31" sqref="M31"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.6328125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="12.6328125" style="1"/>
+    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -763,7 +773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -784,7 +794,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -805,7 +815,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -832,7 +842,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -857,7 +867,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -882,7 +892,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -890,7 +900,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -907,7 +917,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -915,7 +925,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -932,7 +942,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -940,7 +950,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>109</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -957,15 +967,15 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -980,15 +990,15 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1003,15 +1013,15 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1026,15 +1036,15 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1049,15 +1059,15 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1072,15 +1082,15 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1095,9 +1105,9 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>5</v>
@@ -1106,7 +1116,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
@@ -1120,18 +1130,18 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
@@ -1145,9 +1155,9 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>5</v>
@@ -1156,10 +1166,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>14</v>
@@ -1172,21 +1182,21 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>16</v>
@@ -1199,9 +1209,9 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>5</v>
@@ -1210,10 +1220,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>14</v>
@@ -1226,21 +1236,21 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>16</v>
@@ -1253,9 +1263,9 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
@@ -1264,10 +1274,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>14</v>
@@ -1280,21 +1290,21 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>16</v>
@@ -1307,18 +1317,18 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="4">
         <v>321321</v>
@@ -1335,21 +1345,21 @@
         <v>106107</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="4">
         <v>321321</v>
@@ -1366,12 +1376,12 @@
         <v>106107</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -1394,9 +1404,9 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>5</v>
@@ -1419,9 +1429,9 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1433,7 +1443,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3">
@@ -1444,9 +1454,9 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
@@ -1458,7 +1468,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3">
@@ -1469,9 +1479,9 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1483,7 +1493,7 @@
         <v>14</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3">
@@ -1494,9 +1504,9 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>5</v>
@@ -1508,7 +1518,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3">
@@ -1519,9 +1529,9 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
@@ -1533,7 +1543,7 @@
         <v>14</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3">
@@ -1544,9 +1554,9 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -1558,7 +1568,7 @@
         <v>16</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3">
@@ -1569,12 +1579,12 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1583,7 +1593,7 @@
         <v>14</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3">
@@ -1595,15 +1605,15 @@
         <v>106107</v>
       </c>
       <c r="M34" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>108</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1612,7 +1622,7 @@
         <v>16</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
@@ -1624,15 +1634,15 @@
         <v>106107</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>83</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1651,15 +1661,15 @@
         <v>106107</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1678,15 +1688,15 @@
         <v>106107</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1695,7 +1705,7 @@
         <v>14</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -1705,15 +1715,15 @@
         <v>106107</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -1722,7 +1732,7 @@
         <v>16</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -1732,12 +1742,12 @@
         <v>106107</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>5</v>
@@ -1760,9 +1770,9 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>5</v>
@@ -1783,9 +1793,9 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
@@ -1808,9 +1818,9 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>5</v>
@@ -1831,9 +1841,9 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -1858,9 +1868,9 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
@@ -1883,9 +1893,9 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>5</v>
@@ -1910,9 +1920,9 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>5</v>
@@ -1935,9 +1945,9 @@
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>5</v>
@@ -1962,9 +1972,9 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>5</v>
@@ -1987,9 +1997,9 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>5</v>
@@ -2014,9 +2024,9 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>5</v>
@@ -2039,9 +2049,9 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>5</v>
@@ -2064,9 +2074,9 @@
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>5</v>
@@ -2087,9 +2097,9 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>5</v>
@@ -2112,9 +2122,9 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>5</v>
@@ -2135,9 +2145,9 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>5</v>
@@ -2160,9 +2170,9 @@
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>5</v>
@@ -2183,9 +2193,9 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>5</v>
@@ -2208,9 +2218,9 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
add case for query with different data types, also combine with different data sources
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\branches\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF85E62-B145-4089-B5C6-4C3C36B817A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5300128-6EF5-4267-B2E1-4E719E2E2232}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-14570" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="150">
   <si>
     <t>name</t>
   </si>
@@ -361,6 +361,123 @@
   <si>
     <t>motor_current_percent=100.0</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-string-1</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-string-2</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-string-3</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-string-4</t>
+  </si>
+  <si>
+    <t>runid='20190325144526_92b81c0e-4ec9-11e9-a86e-0242ac120004'</t>
+  </si>
+  <si>
+    <t>CIMSOURCE_OPTIMALIZERESULT</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-time-1</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-time-2</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-time-3</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-time-4</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-time-5</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-time-6</t>
+  </si>
+  <si>
+    <t>updateTime&gt;'2021-01-08 00:09:12'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2021-05-21T14:22:43'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2021-01-06T00:15:00'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2021-01-06 00:15:00'</t>
+  </si>
+  <si>
+    <t>updateTime&gt;'2021-01-06T00:15:00'</t>
+  </si>
+  <si>
+    <t>updateTime&gt;'2021-01-06 00:15:00'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-int-1</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-int-2</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-int-3</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-int-4</t>
+  </si>
+  <si>
+    <t>id='1'</t>
+  </si>
+  <si>
+    <t>CIMSOURCE_PREDICTRESULT</t>
+  </si>
+  <si>
+    <t>id='74'</t>
+  </si>
+  <si>
+    <t>optimalizeType='2'</t>
+  </si>
+  <si>
+    <t>train_cfg_timetrg_YN='0'</t>
+  </si>
+  <si>
+    <t>CIMSOURCE_TRAINCONFIG</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-double-1</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-bit-1</t>
+  </si>
+  <si>
+    <t>CIMSOURCE_SIMULATION</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0'</t>
+  </si>
+  <si>
+    <t>lubricate_press_diff='244.1'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-bit-2</t>
+  </si>
+  <si>
+    <t>deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>good request, data retrieved (no scheme check)</t>
+  </si>
+  <si>
+    <t>good request, data retrieved (no scheme check, no condition check)</t>
+  </si>
+  <si>
+    <t>isTraining='true'</t>
+  </si>
+  <si>
+    <t>isTraining=true</t>
   </si>
 </sst>
 </file>
@@ -371,20 +488,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -718,21 +835,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:M76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.69140625" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="12.6640625" style="1"/>
+    <col min="1" max="1" width="30.69140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="49.61328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.53515625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="12.69140625" style="1"/>
+    <col min="6" max="6" width="17.69140625" style="1" customWidth="1"/>
+    <col min="7" max="13" width="12.69140625" style="1"/>
+    <col min="14" max="14" width="36.23046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="12.69140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -773,7 +895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -794,7 +916,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -815,7 +937,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -842,7 +964,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -867,7 +989,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -892,7 +1014,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -917,7 +1039,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -942,7 +1064,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -967,7 +1089,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
@@ -990,7 +1112,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1013,7 +1135,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1036,7 +1158,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1059,7 +1181,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -1082,7 +1204,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
@@ -1105,7 +1227,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -1130,7 +1252,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -1155,7 +1277,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -1182,7 +1304,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
@@ -1209,7 +1331,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
@@ -1236,7 +1358,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
@@ -1263,7 +1385,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
@@ -1290,7 +1412,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
@@ -1317,7 +1439,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>60</v>
       </c>
@@ -1348,7 +1470,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>61</v>
       </c>
@@ -1379,7 +1501,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>63</v>
       </c>
@@ -1404,7 +1526,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>64</v>
       </c>
@@ -1429,7 +1551,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>65</v>
       </c>
@@ -1454,7 +1576,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>66</v>
       </c>
@@ -1479,7 +1601,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>69</v>
       </c>
@@ -1504,7 +1626,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>70</v>
       </c>
@@ -1529,7 +1651,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>73</v>
       </c>
@@ -1554,7 +1676,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>74</v>
       </c>
@@ -1579,7 +1701,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>77</v>
       </c>
@@ -1608,7 +1730,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>78</v>
       </c>
@@ -1637,7 +1759,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>81</v>
       </c>
@@ -1664,7 +1786,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>83</v>
       </c>
@@ -1691,7 +1813,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>84</v>
       </c>
@@ -1718,7 +1840,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>85</v>
       </c>
@@ -1745,7 +1867,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>86</v>
       </c>
@@ -1770,7 +1892,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>87</v>
       </c>
@@ -1793,7 +1915,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>88</v>
       </c>
@@ -1818,7 +1940,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>89</v>
       </c>
@@ -1841,7 +1963,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>90</v>
       </c>
@@ -1868,7 +1990,7 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>91</v>
       </c>
@@ -1893,7 +2015,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>92</v>
       </c>
@@ -1920,7 +2042,7 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>93</v>
       </c>
@@ -1945,7 +2067,7 @@
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>94</v>
       </c>
@@ -1972,7 +2094,7 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
@@ -1997,7 +2119,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>96</v>
       </c>
@@ -2024,7 +2146,7 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>97</v>
       </c>
@@ -2049,7 +2171,7 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>98</v>
       </c>
@@ -2074,7 +2196,7 @@
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>99</v>
       </c>
@@ -2097,7 +2219,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>100</v>
       </c>
@@ -2122,7 +2244,7 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>101</v>
       </c>
@@ -2145,7 +2267,7 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>102</v>
       </c>
@@ -2170,7 +2292,7 @@
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>103</v>
       </c>
@@ -2193,7 +2315,7 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>104</v>
       </c>
@@ -2218,7 +2340,7 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>105</v>
       </c>
@@ -2240,6 +2362,397 @@
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H60" s="1">
+        <v>0</v>
+      </c>
+      <c r="I60" s="1">
+        <v>0</v>
+      </c>
+      <c r="L60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H61" s="1">
+        <v>0</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0</v>
+      </c>
+      <c r="L61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H62" s="1">
+        <v>0</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0</v>
+      </c>
+      <c r="L62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H63" s="1">
+        <v>0</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0</v>
+      </c>
+      <c r="L63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="1">
+        <v>0</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="L64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="1">
+        <v>0</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0</v>
+      </c>
+      <c r="L65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H66" s="1">
+        <v>0</v>
+      </c>
+      <c r="I66" s="1">
+        <v>0</v>
+      </c>
+      <c r="L66" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" s="1">
+        <v>0</v>
+      </c>
+      <c r="I67" s="1">
+        <v>0</v>
+      </c>
+      <c r="L67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" s="1">
+        <v>0</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0</v>
+      </c>
+      <c r="L68" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H69" s="1">
+        <v>0</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0</v>
+      </c>
+      <c r="L69" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H70" s="1">
+        <v>0</v>
+      </c>
+      <c r="I70" s="1">
+        <v>0</v>
+      </c>
+      <c r="L70" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H71" s="1">
+        <v>0</v>
+      </c>
+      <c r="I71" s="1">
+        <v>0</v>
+      </c>
+      <c r="L71" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H72" s="1">
+        <v>0</v>
+      </c>
+      <c r="I72" s="1">
+        <v>10</v>
+      </c>
+      <c r="L72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H73" s="1">
+        <v>0</v>
+      </c>
+      <c r="I73" s="1">
+        <v>0</v>
+      </c>
+      <c r="L73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H74" s="1">
+        <v>1</v>
+      </c>
+      <c r="I74" s="1">
+        <v>2</v>
+      </c>
+      <c r="L74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H75" s="1">
+        <v>0</v>
+      </c>
+      <c r="I75" s="1">
+        <v>0</v>
+      </c>
+      <c r="L75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="H76" s="1">
+        <v>0</v>
+      </c>
+      <c r="I76" s="1">
+        <v>0</v>
+      </c>
+      <c r="L76" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
add cases for cond with different type combination
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF72EF5B-7A15-422E-9B28-34CED6D8D0ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E580BCD4-ED43-4194-A49A-7490CBDAA2F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="206">
   <si>
     <t>name</t>
   </si>
@@ -478,6 +478,174 @@
   </si>
   <si>
     <t>good request, data retrieved (no schema check, no condition check)</t>
+  </si>
+  <si>
+    <t>opt_cfg_emi_frac='0.5'</t>
+  </si>
+  <si>
+    <t>CIMSOURCE_OPTIMALIZECONFIG</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-1</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-String_varchar-1</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-Long_int-1</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-1</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-LocalDateTime_datetime-Long_int-1</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2021-05-21T14:22:43' and id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-String_varchar-Long_int-1</t>
+  </si>
+  <si>
+    <t>deviceName='1#制冷机' and id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-1</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-Long_int-1</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' and id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-String_varchar-Long_int-1</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and deviceName='1#制冷机' and id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-Long_int-1</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机' and id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-Long_int-1</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机' and id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-2</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-String_varchar-2</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-Long_int-2</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-2</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-LocalDateTime_datetime-Long_int-2</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2021-05-21T14:22:43' or id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-String_varchar-Long_int-2</t>
+  </si>
+  <si>
+    <t>deviceName='1#制冷机' or id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-2</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-Long_int-2</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43' or id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-String_varchar-Long_int-2</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or deviceName='1#制冷机' or id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-Long_int-2</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机' or id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-Long_int-2</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机' or id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-3</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-Long_int-3</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' or id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-String_varchar-Long_int-3</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or deviceName='1#制冷机' and id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-Long_int-3</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机' and id='38'</t>
+  </si>
+  <si>
+    <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-Long_int-3</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机' or id='38'</t>
   </si>
 </sst>
 </file>
@@ -835,16 +1003,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
-  <dimension ref="A1:M76"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69140625" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.69140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="54.53515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="49.61328125" style="1" customWidth="1"/>
     <col min="3" max="3" width="38.53515625" style="1" customWidth="1"/>
     <col min="4" max="5" width="12.69140625" style="1"/>
@@ -2693,10 +2861,10 @@
         <v>148</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="H74" s="1">
         <v>1</v>
@@ -2751,6 +2919,627 @@
         <v>0</v>
       </c>
       <c r="L76" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H77" s="1">
+        <v>0</v>
+      </c>
+      <c r="I77" s="1">
+        <v>0</v>
+      </c>
+      <c r="L77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H78" s="1">
+        <v>0</v>
+      </c>
+      <c r="I78" s="1">
+        <v>0</v>
+      </c>
+      <c r="L78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H79" s="1">
+        <v>0</v>
+      </c>
+      <c r="I79" s="1">
+        <v>0</v>
+      </c>
+      <c r="L79" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H80" s="1">
+        <v>0</v>
+      </c>
+      <c r="I80" s="1">
+        <v>0</v>
+      </c>
+      <c r="L80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H81" s="1">
+        <v>0</v>
+      </c>
+      <c r="I81" s="1">
+        <v>0</v>
+      </c>
+      <c r="L81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H82" s="1">
+        <v>0</v>
+      </c>
+      <c r="I82" s="1">
+        <v>0</v>
+      </c>
+      <c r="L82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H83" s="1">
+        <v>0</v>
+      </c>
+      <c r="I83" s="1">
+        <v>0</v>
+      </c>
+      <c r="L83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H84" s="1">
+        <v>0</v>
+      </c>
+      <c r="I84" s="1">
+        <v>0</v>
+      </c>
+      <c r="L84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H85" s="1">
+        <v>0</v>
+      </c>
+      <c r="I85" s="1">
+        <v>0</v>
+      </c>
+      <c r="L85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H86" s="1">
+        <v>0</v>
+      </c>
+      <c r="I86" s="1">
+        <v>0</v>
+      </c>
+      <c r="L86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H87" s="1">
+        <v>0</v>
+      </c>
+      <c r="I87" s="1">
+        <v>0</v>
+      </c>
+      <c r="L87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H88" s="1">
+        <v>0</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0</v>
+      </c>
+      <c r="L88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0</v>
+      </c>
+      <c r="I89" s="1">
+        <v>0</v>
+      </c>
+      <c r="L89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H90" s="1">
+        <v>0</v>
+      </c>
+      <c r="I90" s="1">
+        <v>0</v>
+      </c>
+      <c r="L90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H91" s="1">
+        <v>0</v>
+      </c>
+      <c r="I91" s="1">
+        <v>0</v>
+      </c>
+      <c r="L91" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H92" s="1">
+        <v>0</v>
+      </c>
+      <c r="I92" s="1">
+        <v>0</v>
+      </c>
+      <c r="L92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H93" s="1">
+        <v>0</v>
+      </c>
+      <c r="I93" s="1">
+        <v>0</v>
+      </c>
+      <c r="L93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H94" s="1">
+        <v>0</v>
+      </c>
+      <c r="I94" s="1">
+        <v>0</v>
+      </c>
+      <c r="L94" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H95" s="1">
+        <v>0</v>
+      </c>
+      <c r="I95" s="1">
+        <v>0</v>
+      </c>
+      <c r="L95" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H96" s="1">
+        <v>0</v>
+      </c>
+      <c r="I96" s="1">
+        <v>0</v>
+      </c>
+      <c r="L96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H97" s="1">
+        <v>0</v>
+      </c>
+      <c r="I97" s="1">
+        <v>0</v>
+      </c>
+      <c r="L97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H98" s="1">
+        <v>0</v>
+      </c>
+      <c r="I98" s="1">
+        <v>0</v>
+      </c>
+      <c r="L98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H99" s="1">
+        <v>0</v>
+      </c>
+      <c r="I99" s="1">
+        <v>0</v>
+      </c>
+      <c r="L99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H100" s="1">
+        <v>0</v>
+      </c>
+      <c r="I100" s="1">
+        <v>0</v>
+      </c>
+      <c r="L100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H101" s="1">
+        <v>0</v>
+      </c>
+      <c r="I101" s="1">
+        <v>0</v>
+      </c>
+      <c r="L101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H102" s="1">
+        <v>0</v>
+      </c>
+      <c r="I102" s="1">
+        <v>0</v>
+      </c>
+      <c r="L102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H103" s="1">
+        <v>0</v>
+      </c>
+      <c r="I103" s="1">
+        <v>0</v>
+      </c>
+      <c r="L103" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update iems connector test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E580BCD4-ED43-4194-A49A-7490CBDAA2F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB51548E-38D7-4451-A0A9-A73081F41E17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -375,9 +375,6 @@
     <t>iems-connector-test-mysql-string-4</t>
   </si>
   <si>
-    <t>runid='20190325144526_92b81c0e-4ec9-11e9-a86e-0242ac120004'</t>
-  </si>
-  <si>
     <t>CIMSOURCE_OPTIMALIZERESULT</t>
   </si>
   <si>
@@ -435,9 +432,6 @@
     <t>CIMSOURCE_PREDICTRESULT</t>
   </si>
   <si>
-    <t>id='74'</t>
-  </si>
-  <si>
     <t>optimalizeType='2'</t>
   </si>
   <si>
@@ -646,6 +640,12 @@
   </si>
   <si>
     <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机' or id='38'</t>
+  </si>
+  <si>
+    <t>runid='20210526141938_1_5993b5b8-bdea-11eb-a875-0242ac120005'</t>
+  </si>
+  <si>
+    <t>id='2267'</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1006,8 @@
   <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69140625" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -2536,10 +2536,10 @@
         <v>111</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>16</v>
@@ -2559,10 +2559,10 @@
         <v>112</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>16</v>
@@ -2582,10 +2582,10 @@
         <v>113</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>16</v>
@@ -2605,13 +2605,13 @@
         <v>114</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="H63" s="1">
         <v>0</v>
@@ -2625,13 +2625,13 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>16</v>
@@ -2648,13 +2648,13 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>16</v>
@@ -2671,13 +2671,13 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>14</v>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>14</v>
@@ -2717,13 +2717,13 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>14</v>
@@ -2740,13 +2740,13 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>14</v>
@@ -2763,16 +2763,16 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="H70" s="1">
         <v>0</v>
@@ -2786,16 +2786,16 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>135</v>
+        <v>205</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H71" s="1">
         <v>0</v>
@@ -2809,16 +2809,16 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H72" s="1">
         <v>0</v>
@@ -2832,16 +2832,16 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H73" s="1">
         <v>0</v>
@@ -2855,16 +2855,16 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="F74" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H74" s="1">
         <v>1</v>
@@ -2878,16 +2878,16 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H75" s="1">
         <v>0</v>
@@ -2901,16 +2901,16 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H76" s="1">
         <v>0</v>
@@ -2924,13 +2924,13 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>16</v>
@@ -2947,13 +2947,13 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>16</v>
@@ -2970,13 +2970,13 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>16</v>
@@ -2993,13 +2993,13 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>16</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>16</v>
@@ -3039,13 +3039,13 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>16</v>
@@ -3062,13 +3062,13 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>16</v>
@@ -3085,13 +3085,13 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>16</v>
@@ -3108,13 +3108,13 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>16</v>
@@ -3131,13 +3131,13 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>16</v>
@@ -3154,13 +3154,13 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>16</v>
@@ -3177,13 +3177,13 @@
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>16</v>
@@ -3200,13 +3200,13 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>16</v>
@@ -3223,13 +3223,13 @@
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>16</v>
@@ -3246,13 +3246,13 @@
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>16</v>
@@ -3269,13 +3269,13 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>16</v>
@@ -3292,13 +3292,13 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>16</v>
@@ -3315,13 +3315,13 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>16</v>
@@ -3338,13 +3338,13 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>16</v>
@@ -3361,13 +3361,13 @@
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>16</v>
@@ -3384,13 +3384,13 @@
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>16</v>
@@ -3407,13 +3407,13 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>16</v>
@@ -3430,13 +3430,13 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>16</v>
@@ -3453,13 +3453,13 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>16</v>
@@ -3476,13 +3476,13 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>16</v>
@@ -3499,13 +3499,13 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>16</v>
@@ -3522,13 +3522,13 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
update iems connector cases
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C56CAB-00AE-4DB1-AB02-3BA8ED0956C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BC45D5-A625-49DF-A80A-3A69F06C1F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -402,12 +402,6 @@
     <t>updateTime&lt;'2021-05-21T14:22:43'</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-01-06T00:15:00'</t>
-  </si>
-  <si>
-    <t>updateTime&lt;'2021-01-06 00:15:00'</t>
-  </si>
-  <si>
     <t>updateTime&gt;'2021-01-06T00:15:00'</t>
   </si>
   <si>
@@ -646,6 +640,12 @@
   </si>
   <si>
     <t>id='2267'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2022-01-06T00:15:00'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2022-01-06 00:15:00'</t>
   </si>
 </sst>
 </file>
@@ -1007,22 +1007,22 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C71" sqref="C71"/>
+      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.69140625" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="54.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="49.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.5546875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="12.6640625" style="1"/>
-    <col min="6" max="6" width="17.6640625" style="1" customWidth="1"/>
-    <col min="7" max="13" width="12.6640625" style="1"/>
-    <col min="14" max="14" width="36.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="12.6640625" style="1"/>
+    <col min="1" max="1" width="54.53515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="49.69140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.53515625" style="1" customWidth="1"/>
+    <col min="4" max="5" width="12.69140625" style="1"/>
+    <col min="6" max="6" width="17.69140625" style="1" customWidth="1"/>
+    <col min="7" max="13" width="12.69140625" style="1"/>
+    <col min="14" max="14" width="36.23046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="12.69140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1084,7 +1084,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1232,7 +1232,7 @@
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1257,7 +1257,7 @@
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
@@ -1280,7 +1280,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1303,7 +1303,7 @@
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1326,7 +1326,7 @@
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>38</v>
       </c>
@@ -1349,7 +1349,7 @@
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -1372,7 +1372,7 @@
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
@@ -1395,7 +1395,7 @@
       <c r="L15" s="3"/>
       <c r="M15" s="3"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -1420,7 +1420,7 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>48</v>
       </c>
@@ -1472,7 +1472,7 @@
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>50</v>
       </c>
@@ -1499,7 +1499,7 @@
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>53</v>
       </c>
@@ -1526,7 +1526,7 @@
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>54</v>
       </c>
@@ -1553,7 +1553,7 @@
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>55</v>
       </c>
@@ -1580,7 +1580,7 @@
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>56</v>
       </c>
@@ -1607,7 +1607,7 @@
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>60</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>61</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>63</v>
       </c>
@@ -1694,7 +1694,7 @@
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>64</v>
       </c>
@@ -1719,7 +1719,7 @@
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>65</v>
       </c>
@@ -1744,7 +1744,7 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>66</v>
       </c>
@@ -1769,7 +1769,7 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>69</v>
       </c>
@@ -1794,7 +1794,7 @@
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>70</v>
       </c>
@@ -1819,7 +1819,7 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>73</v>
       </c>
@@ -1844,7 +1844,7 @@
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>74</v>
       </c>
@@ -1869,7 +1869,7 @@
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>77</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>78</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>81</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>83</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>84</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>85</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>86</v>
       </c>
@@ -2060,7 +2060,7 @@
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>87</v>
       </c>
@@ -2083,7 +2083,7 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>88</v>
       </c>
@@ -2108,7 +2108,7 @@
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>89</v>
       </c>
@@ -2131,7 +2131,7 @@
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>90</v>
       </c>
@@ -2158,7 +2158,7 @@
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>91</v>
       </c>
@@ -2183,7 +2183,7 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>92</v>
       </c>
@@ -2210,7 +2210,7 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>93</v>
       </c>
@@ -2235,7 +2235,7 @@
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>94</v>
       </c>
@@ -2262,7 +2262,7 @@
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>95</v>
       </c>
@@ -2287,7 +2287,7 @@
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>96</v>
       </c>
@@ -2314,7 +2314,7 @@
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>97</v>
       </c>
@@ -2339,7 +2339,7 @@
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>98</v>
       </c>
@@ -2364,7 +2364,7 @@
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>99</v>
       </c>
@@ -2387,7 +2387,7 @@
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>100</v>
       </c>
@@ -2412,7 +2412,7 @@
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>101</v>
       </c>
@@ -2435,7 +2435,7 @@
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>102</v>
       </c>
@@ -2460,7 +2460,7 @@
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>103</v>
       </c>
@@ -2483,7 +2483,7 @@
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>104</v>
       </c>
@@ -2508,7 +2508,7 @@
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>105</v>
       </c>
@@ -2531,15 +2531,15 @@
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -2560,15 +2560,15 @@
       </c>
       <c r="M60" s="3"/>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>112</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -2589,15 +2589,15 @@
       </c>
       <c r="M61" s="3"/>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -2618,15 +2618,15 @@
       </c>
       <c r="M62" s="3"/>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>114</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -2647,12 +2647,12 @@
       </c>
       <c r="M63" s="3"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>122</v>
@@ -2676,12 +2676,12 @@
       </c>
       <c r="M64" s="3"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>123</v>
@@ -2705,15 +2705,15 @@
       </c>
       <c r="M65" s="3"/>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>124</v>
+        <v>204</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -2734,15 +2734,15 @@
       </c>
       <c r="M66" s="3"/>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>119</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>125</v>
+        <v>205</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -2763,15 +2763,15 @@
       </c>
       <c r="M67" s="3"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>120</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -2792,15 +2792,15 @@
       </c>
       <c r="M68" s="3"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>121</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -2821,20 +2821,20 @@
       </c>
       <c r="M69" s="3"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3">
@@ -2850,15 +2850,15 @@
       </c>
       <c r="M70" s="3"/>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -2879,15 +2879,15 @@
       </c>
       <c r="M71" s="3"/>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
@@ -2908,20 +2908,20 @@
       </c>
       <c r="M72" s="3"/>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3">
@@ -2937,20 +2937,20 @@
       </c>
       <c r="M73" s="3"/>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3">
@@ -2966,20 +2966,20 @@
       </c>
       <c r="M74" s="3"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3">
@@ -2995,20 +2995,20 @@
       </c>
       <c r="M75" s="3"/>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3">
@@ -3024,15 +3024,15 @@
       </c>
       <c r="M76" s="3"/>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -3053,15 +3053,15 @@
       </c>
       <c r="M77" s="3"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
@@ -3082,15 +3082,15 @@
       </c>
       <c r="M78" s="3"/>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -3111,15 +3111,15 @@
       </c>
       <c r="M79" s="3"/>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -3140,15 +3140,15 @@
       </c>
       <c r="M80" s="3"/>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -3169,15 +3169,15 @@
       </c>
       <c r="M81" s="3"/>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -3198,15 +3198,15 @@
       </c>
       <c r="M82" s="3"/>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -3227,15 +3227,15 @@
       </c>
       <c r="M83" s="3"/>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
@@ -3256,15 +3256,15 @@
       </c>
       <c r="M84" s="3"/>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -3285,15 +3285,15 @@
       </c>
       <c r="M85" s="3"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -3314,15 +3314,15 @@
       </c>
       <c r="M86" s="3"/>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -3343,15 +3343,15 @@
       </c>
       <c r="M87" s="3"/>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
@@ -3372,15 +3372,15 @@
       </c>
       <c r="M88" s="3"/>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
@@ -3401,15 +3401,15 @@
       </c>
       <c r="M89" s="3"/>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -3430,15 +3430,15 @@
       </c>
       <c r="M90" s="3"/>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -3459,15 +3459,15 @@
       </c>
       <c r="M91" s="3"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
@@ -3488,15 +3488,15 @@
       </c>
       <c r="M92" s="3"/>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
@@ -3517,15 +3517,15 @@
       </c>
       <c r="M93" s="3"/>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
@@ -3546,15 +3546,15 @@
       </c>
       <c r="M94" s="3"/>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
@@ -3575,15 +3575,15 @@
       </c>
       <c r="M95" s="3"/>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
@@ -3604,15 +3604,15 @@
       </c>
       <c r="M96" s="3"/>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
@@ -3633,15 +3633,15 @@
       </c>
       <c r="M97" s="3"/>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
@@ -3662,15 +3662,15 @@
       </c>
       <c r="M98" s="3"/>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
@@ -3691,15 +3691,15 @@
       </c>
       <c r="M99" s="3"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
@@ -3720,15 +3720,15 @@
       </c>
       <c r="M100" s="3"/>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
@@ -3749,15 +3749,15 @@
       </c>
       <c r="M101" s="3"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
@@ -3778,15 +3778,15 @@
       </c>
       <c r="M102" s="3"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>

</xml_diff>

<commit_message>
sync coneector xlsx files from feature-with-comment to feature-backup
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BC45D5-A625-49DF-A80A-3A69F06C1F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BBD1E3-0FC5-4D57-B578-52229A3D5A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>searchData.name is not valid,reason: must not be blank</t>
   </si>
   <si>
-    <t>The m2 service unavailable: (request M2 failed : no found entity ).</t>
-  </si>
-  <si>
     <t>Siid</t>
   </si>
   <si>
@@ -399,9 +396,6 @@
     <t>updateTime&gt;'2021-01-08 00:09:12'</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43'</t>
-  </si>
-  <si>
     <t>updateTime&gt;'2021-01-06T00:15:00'</t>
   </si>
   <si>
@@ -477,9 +471,6 @@
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-String_varchar-1</t>
   </si>
   <si>
@@ -489,63 +480,33 @@
     <t>iems-connector-test-mysql-Float_varchar-Long_int-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-1</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-LocalDateTime_datetime-Long_int-1</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-String_varchar-Long_int-1</t>
   </si>
   <si>
-    <t>deviceName='1#制冷机' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-Long_int-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-String_varchar-Long_int-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and deviceName='1#制冷机' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-Long_int-1</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-Long_int-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-2</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-String_varchar-2</t>
   </si>
   <si>
@@ -555,33 +516,18 @@
     <t>iems-connector-test-mysql-Float_varchar-Long_int-2</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' or id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-2</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-LocalDateTime_datetime-Long_int-2</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' or id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-String_varchar-Long_int-2</t>
   </si>
   <si>
-    <t>deviceName='1#制冷机' or id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-2</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-Long_int-2</t>
   </si>
   <si>
@@ -615,9 +561,6 @@
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-Long_int-3</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' or id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-String_varchar-Long_int-3</t>
   </si>
   <si>
@@ -627,25 +570,82 @@
     <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-Long_int-3</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-Long_int-3</t>
   </si>
   <si>
     <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机' or id='38'</t>
   </si>
   <si>
-    <t>runid='20210526141938_1_5993b5b8-bdea-11eb-a875-0242ac120005'</t>
-  </si>
-  <si>
-    <t>id='2267'</t>
-  </si>
-  <si>
     <t>updateTime&lt;'2022-01-06T00:15:00'</t>
   </si>
   <si>
     <t>updateTime&lt;'2022-01-06 00:15:00'</t>
+  </si>
+  <si>
+    <t>[add domain entities for mapping success] info = [[iEMS], 12321])</t>
+  </si>
+  <si>
+    <t>runid='20211202140114_1_41b809d6-5335-11ec-8833-0242ac12000f'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43'</t>
+  </si>
+  <si>
+    <t>id='46'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2025-05-21T14:22:43'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and id='10100'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' and deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' and id='10100'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2025-05-21T14:22:43' and deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and deviceName='1#制冷机' and id='10100'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' and deviceName='1#制冷机' and id='10100'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2025-05-21T14:22:43' and deviceName='1#制冷机' and id='10100'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or updateTime&lt;'2025-05-21T14:22:43'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or id='10100'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' or deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' or id='10100'</t>
+  </si>
+  <si>
+    <t>deviceName='1#制冷机' or id='10100'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or updateTime&lt;'2025-05-21T14:22:43' or deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' or id='10100'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' or deviceName='1#制冷机' and id='38'</t>
+  </si>
+  <si>
+    <t>deviceName='1#制冷机' and id='10100'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2025-05-21T14:22:43' and id='10100'</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1006,8 @@
   <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69140625" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -1151,10 +1151,10 @@
       <c r="J5" s="3"/>
       <c r="K5" s="4"/>
       <c r="L5" s="3">
-        <v>108001</v>
+        <v>106920</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -1173,7 +1173,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1190,7 +1190,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1198,7 +1198,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1215,7 +1215,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1223,7 +1223,7 @@
         <v>14</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1240,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1248,7 +1248,7 @@
         <v>16</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1259,13 +1259,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1282,13 +1282,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1305,13 +1305,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1328,13 +1328,13 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1351,13 +1351,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1374,13 +1374,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>5</v>
@@ -1406,7 +1406,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
@@ -1422,16 +1422,16 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
@@ -1447,7 +1447,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>5</v>
@@ -1456,10 +1456,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>14</v>
@@ -1474,19 +1474,19 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>16</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>5</v>
@@ -1510,10 +1510,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>14</v>
@@ -1528,19 +1528,19 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>16</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
@@ -1564,10 +1564,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>14</v>
@@ -1582,19 +1582,19 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>16</v>
@@ -1609,16 +1609,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="4">
         <v>321321</v>
@@ -1635,21 +1635,21 @@
         <v>106107</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="4">
         <v>321321</v>
@@ -1666,12 +1666,12 @@
         <v>106107</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -1683,7 +1683,7 @@
         <v>14</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3">
@@ -1696,7 +1696,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>5</v>
@@ -1708,7 +1708,7 @@
         <v>16</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3">
@@ -1721,7 +1721,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1733,7 +1733,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3">
@@ -1746,7 +1746,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
@@ -1758,7 +1758,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3">
@@ -1771,7 +1771,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1783,7 +1783,7 @@
         <v>14</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3">
@@ -1796,7 +1796,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>5</v>
@@ -1808,7 +1808,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3">
@@ -1821,7 +1821,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
@@ -1833,7 +1833,7 @@
         <v>14</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3">
@@ -1846,7 +1846,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -1858,7 +1858,7 @@
         <v>16</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3">
@@ -1871,10 +1871,10 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1883,7 +1883,7 @@
         <v>14</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3">
@@ -1895,15 +1895,15 @@
         <v>106107</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1912,7 +1912,7 @@
         <v>16</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
@@ -1924,15 +1924,15 @@
         <v>106107</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1951,15 +1951,15 @@
         <v>106107</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1978,15 +1978,15 @@
         <v>106107</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1995,7 +1995,7 @@
         <v>14</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -2005,15 +2005,15 @@
         <v>106107</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2022,7 +2022,7 @@
         <v>16</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -2032,12 +2032,12 @@
         <v>106107</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>5</v>
@@ -2049,7 +2049,7 @@
         <v>14</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H40" s="3">
         <v>0</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>5</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
@@ -2097,7 +2097,7 @@
         <v>14</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3">
@@ -2110,7 +2110,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>5</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -2145,7 +2145,7 @@
         <v>14</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H44" s="3">
         <v>0</v>
@@ -2160,7 +2160,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>5</v>
@@ -2197,7 +2197,7 @@
         <v>14</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H46" s="3">
         <v>2</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>5</v>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>5</v>
@@ -2249,7 +2249,7 @@
         <v>14</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H48" s="3">
         <v>-2</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>5</v>
@@ -2289,7 +2289,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>5</v>
@@ -2301,7 +2301,7 @@
         <v>14</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H50" s="3">
         <v>2</v>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>5</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>5</v>
@@ -2353,7 +2353,7 @@
         <v>14</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H52" s="3">
         <v>2</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>5</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>5</v>
@@ -2401,7 +2401,7 @@
         <v>14</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H54" s="3">
         <v>-2</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>5</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>5</v>
@@ -2449,7 +2449,7 @@
         <v>14</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H56" s="3"/>
       <c r="I56" s="3">
@@ -2462,7 +2462,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>5</v>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>5</v>
@@ -2497,7 +2497,7 @@
         <v>14</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="3">
@@ -2510,7 +2510,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>5</v>
@@ -2533,13 +2533,13 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -2562,13 +2562,13 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -2591,13 +2591,13 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -2620,18 +2620,18 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3">
@@ -2649,13 +2649,13 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -2678,13 +2678,13 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -2707,13 +2707,13 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -2765,13 +2765,13 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -2794,13 +2794,13 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -2823,18 +2823,18 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3">
@@ -2852,18 +2852,18 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3">
@@ -2881,18 +2881,18 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3">
@@ -2910,18 +2910,18 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3">
@@ -2939,18 +2939,18 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3">
@@ -2968,18 +2968,18 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3">
@@ -2997,18 +2997,18 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3">
@@ -3026,13 +3026,13 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>149</v>
+        <v>188</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -3055,13 +3055,13 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
@@ -3084,13 +3084,13 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -3113,13 +3113,13 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -3171,13 +3171,13 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -3200,13 +3200,13 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -3229,13 +3229,13 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
@@ -3258,13 +3258,13 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -3287,13 +3287,13 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -3316,13 +3316,13 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -3345,13 +3345,13 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
@@ -3374,13 +3374,13 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
@@ -3403,13 +3403,13 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -3432,13 +3432,13 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -3461,13 +3461,13 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
@@ -3490,13 +3490,13 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
@@ -3519,13 +3519,13 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
@@ -3548,13 +3548,13 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
@@ -3577,13 +3577,13 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
@@ -3606,13 +3606,13 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
@@ -3635,13 +3635,13 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
@@ -3664,13 +3664,13 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
@@ -3693,13 +3693,13 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
@@ -3722,13 +3722,13 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
@@ -3751,13 +3751,13 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
@@ -3780,13 +3780,13 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>

</xml_diff>

<commit_message>
add test case for connector realtime
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BC45D5-A625-49DF-A80A-3A69F06C1F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BBD1E3-0FC5-4D57-B578-52229A3D5A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -114,9 +114,6 @@
     <t>searchData.name is not valid,reason: must not be blank</t>
   </si>
   <si>
-    <t>The m2 service unavailable: (request M2 failed : no found entity ).</t>
-  </si>
-  <si>
     <t>Siid</t>
   </si>
   <si>
@@ -399,9 +396,6 @@
     <t>updateTime&gt;'2021-01-08 00:09:12'</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43'</t>
-  </si>
-  <si>
     <t>updateTime&gt;'2021-01-06T00:15:00'</t>
   </si>
   <si>
@@ -477,9 +471,6 @@
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-String_varchar-1</t>
   </si>
   <si>
@@ -489,63 +480,33 @@
     <t>iems-connector-test-mysql-Float_varchar-Long_int-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-1</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-LocalDateTime_datetime-Long_int-1</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-String_varchar-Long_int-1</t>
   </si>
   <si>
-    <t>deviceName='1#制冷机' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-Long_int-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-String_varchar-Long_int-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and deviceName='1#制冷机' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-Long_int-1</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-Long_int-1</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-2</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-String_varchar-2</t>
   </si>
   <si>
@@ -555,33 +516,18 @@
     <t>iems-connector-test-mysql-Float_varchar-Long_int-2</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' or id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-2</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-LocalDateTime_datetime-Long_int-2</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' or id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-String_varchar-Long_int-2</t>
   </si>
   <si>
-    <t>deviceName='1#制冷机' or id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-2</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-Long_int-2</t>
   </si>
   <si>
@@ -615,9 +561,6 @@
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-Long_int-3</t>
   </si>
   <si>
-    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' or id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-String_varchar-Long_int-3</t>
   </si>
   <si>
@@ -627,25 +570,82 @@
     <t>iems-connector-test-mysql-LocalDateTime_datetime-String_varchar-Long_int-3</t>
   </si>
   <si>
-    <t>updateTime&lt;'2021-05-21T14:22:43' or deviceName='1#制冷机' and id='38'</t>
-  </si>
-  <si>
     <t>iems-connector-test-mysql-Float_varchar-LocalDateTime_datetime-String_varchar-Long_int-3</t>
   </si>
   <si>
     <t>motor_current_percent='92.0' or updateTime&lt;'2021-05-21T14:22:43' and deviceName='1#制冷机' or id='38'</t>
   </si>
   <si>
-    <t>runid='20210526141938_1_5993b5b8-bdea-11eb-a875-0242ac120005'</t>
-  </si>
-  <si>
-    <t>id='2267'</t>
-  </si>
-  <si>
     <t>updateTime&lt;'2022-01-06T00:15:00'</t>
   </si>
   <si>
     <t>updateTime&lt;'2022-01-06 00:15:00'</t>
+  </si>
+  <si>
+    <t>[add domain entities for mapping success] info = [[iEMS], 12321])</t>
+  </si>
+  <si>
+    <t>runid='20211202140114_1_41b809d6-5335-11ec-8833-0242ac12000f'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43'</t>
+  </si>
+  <si>
+    <t>id='46'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2025-05-21T14:22:43'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and id='10100'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' and deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' and id='10100'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2025-05-21T14:22:43' and deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and deviceName='1#制冷机' and id='10100'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' and deviceName='1#制冷机' and id='10100'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2025-05-21T14:22:43' and deviceName='1#制冷机' and id='10100'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or updateTime&lt;'2025-05-21T14:22:43'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or id='10100'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' or deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' or id='10100'</t>
+  </si>
+  <si>
+    <t>deviceName='1#制冷机' or id='10100'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' or updateTime&lt;'2025-05-21T14:22:43' or deviceName='1#制冷机'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2021-05-21T14:22:43' or id='10100'</t>
+  </si>
+  <si>
+    <t>updateTime&lt;'2025-05-21T14:22:43' or deviceName='1#制冷机' and id='38'</t>
+  </si>
+  <si>
+    <t>deviceName='1#制冷机' and id='10100'</t>
+  </si>
+  <si>
+    <t>motor_current_percent='92.0' and updateTime&lt;'2025-05-21T14:22:43' and id='10100'</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1006,8 @@
   <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C67" sqref="C67"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69140625" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -1151,10 +1151,10 @@
       <c r="J5" s="3"/>
       <c r="K5" s="4"/>
       <c r="L5" s="3">
-        <v>108001</v>
+        <v>106920</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>29</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -1173,7 +1173,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -1190,7 +1190,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1198,7 +1198,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -1215,7 +1215,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1223,7 +1223,7 @@
         <v>14</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1240,7 +1240,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1248,7 +1248,7 @@
         <v>16</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -1259,13 +1259,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -1282,13 +1282,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1305,13 +1305,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -1328,13 +1328,13 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1351,13 +1351,13 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1374,13 +1374,13 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C15" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1397,7 +1397,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>5</v>
@@ -1406,7 +1406,7 @@
         <v>21</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3" t="s">
@@ -1422,16 +1422,16 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3" t="s">
@@ -1447,7 +1447,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>5</v>
@@ -1456,10 +1456,10 @@
         <v>21</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>14</v>
@@ -1474,19 +1474,19 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>16</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>5</v>
@@ -1510,10 +1510,10 @@
         <v>21</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>14</v>
@@ -1528,19 +1528,19 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>16</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
@@ -1564,10 +1564,10 @@
         <v>21</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>14</v>
@@ -1582,19 +1582,19 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>16</v>
@@ -1609,16 +1609,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>21</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" s="4">
         <v>321321</v>
@@ -1635,21 +1635,21 @@
         <v>106107</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" s="4">
         <v>321321</v>
@@ -1666,12 +1666,12 @@
         <v>106107</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -1683,7 +1683,7 @@
         <v>14</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3">
@@ -1696,7 +1696,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>5</v>
@@ -1708,7 +1708,7 @@
         <v>16</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3">
@@ -1721,7 +1721,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1733,7 +1733,7 @@
         <v>14</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3">
@@ -1746,7 +1746,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>5</v>
@@ -1758,7 +1758,7 @@
         <v>16</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3">
@@ -1771,7 +1771,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1783,7 +1783,7 @@
         <v>14</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3">
@@ -1796,7 +1796,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>5</v>
@@ -1808,7 +1808,7 @@
         <v>16</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3">
@@ -1821,7 +1821,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>5</v>
@@ -1833,7 +1833,7 @@
         <v>14</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3">
@@ -1846,7 +1846,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>5</v>
@@ -1858,7 +1858,7 @@
         <v>16</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3">
@@ -1871,10 +1871,10 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1883,7 +1883,7 @@
         <v>14</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3">
@@ -1895,15 +1895,15 @@
         <v>106107</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1912,7 +1912,7 @@
         <v>16</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3">
@@ -1924,15 +1924,15 @@
         <v>106107</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>82</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1951,15 +1951,15 @@
         <v>106107</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -1978,15 +1978,15 @@
         <v>106107</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -1995,7 +1995,7 @@
         <v>14</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
@@ -2005,15 +2005,15 @@
         <v>106107</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2022,7 +2022,7 @@
         <v>16</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
@@ -2032,12 +2032,12 @@
         <v>106107</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>5</v>
@@ -2049,7 +2049,7 @@
         <v>14</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H40" s="3">
         <v>0</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>5</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>5</v>
@@ -2097,7 +2097,7 @@
         <v>14</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H42" s="3"/>
       <c r="I42" s="3">
@@ -2110,7 +2110,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>5</v>
@@ -2133,7 +2133,7 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>5</v>
@@ -2145,7 +2145,7 @@
         <v>14</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H44" s="3">
         <v>0</v>
@@ -2160,7 +2160,7 @@
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>5</v>
@@ -2185,7 +2185,7 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>5</v>
@@ -2197,7 +2197,7 @@
         <v>14</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H46" s="3">
         <v>2</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>5</v>
@@ -2237,7 +2237,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>5</v>
@@ -2249,7 +2249,7 @@
         <v>14</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H48" s="3">
         <v>-2</v>
@@ -2264,7 +2264,7 @@
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>5</v>
@@ -2289,7 +2289,7 @@
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>5</v>
@@ -2301,7 +2301,7 @@
         <v>14</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H50" s="3">
         <v>2</v>
@@ -2316,7 +2316,7 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>5</v>
@@ -2341,7 +2341,7 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>5</v>
@@ -2353,7 +2353,7 @@
         <v>14</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H52" s="3">
         <v>2</v>
@@ -2366,7 +2366,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>5</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>5</v>
@@ -2401,7 +2401,7 @@
         <v>14</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H54" s="3">
         <v>-2</v>
@@ -2414,7 +2414,7 @@
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>5</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>5</v>
@@ -2449,7 +2449,7 @@
         <v>14</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H56" s="3"/>
       <c r="I56" s="3">
@@ -2462,7 +2462,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>5</v>
@@ -2485,7 +2485,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>5</v>
@@ -2497,7 +2497,7 @@
         <v>14</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H58" s="3"/>
       <c r="I58" s="3">
@@ -2510,7 +2510,7 @@
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>5</v>
@@ -2533,13 +2533,13 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -2562,13 +2562,13 @@
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -2591,13 +2591,13 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
@@ -2620,18 +2620,18 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3">
@@ -2649,13 +2649,13 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -2678,13 +2678,13 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>123</v>
+        <v>186</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -2707,13 +2707,13 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -2736,13 +2736,13 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -2765,13 +2765,13 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
@@ -2794,13 +2794,13 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
@@ -2823,18 +2823,18 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3">
@@ -2852,18 +2852,18 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3">
@@ -2881,18 +2881,18 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3">
@@ -2910,18 +2910,18 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3">
@@ -2939,18 +2939,18 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B74" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3">
@@ -2968,18 +2968,18 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3">
@@ -2997,18 +2997,18 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3">
@@ -3026,13 +3026,13 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>149</v>
+        <v>188</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -3055,13 +3055,13 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
@@ -3084,13 +3084,13 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -3113,13 +3113,13 @@
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -3142,13 +3142,13 @@
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>157</v>
+        <v>191</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -3171,13 +3171,13 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -3200,13 +3200,13 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>161</v>
+        <v>192</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -3229,13 +3229,13 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
@@ -3258,13 +3258,13 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>165</v>
+        <v>193</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -3287,13 +3287,13 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -3316,13 +3316,13 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>169</v>
+        <v>195</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -3345,13 +3345,13 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
@@ -3374,13 +3374,13 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
@@ -3403,13 +3403,13 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -3432,13 +3432,13 @@
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -3461,13 +3461,13 @@
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
@@ -3490,13 +3490,13 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
@@ -3519,13 +3519,13 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>183</v>
+        <v>201</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
@@ -3548,13 +3548,13 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
@@ -3577,13 +3577,13 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
@@ -3606,13 +3606,13 @@
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
@@ -3635,13 +3635,13 @@
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
@@ -3664,13 +3664,13 @@
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
@@ -3693,13 +3693,13 @@
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
@@ -3722,13 +3722,13 @@
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
@@ -3751,13 +3751,13 @@
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
@@ -3780,13 +3780,13 @@
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>

</xml_diff>

<commit_message>
update iems-connector-test-data.xlsx and iems-entity-management-test-data.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BBD1E3-0FC5-4D57-B578-52229A3D5A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8C18B3-4BDB-4AF3-9EEB-1E3BA68B6936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-129" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="2" r:id="rId1"/>
@@ -582,9 +582,6 @@
     <t>updateTime&lt;'2022-01-06 00:15:00'</t>
   </si>
   <si>
-    <t>[add domain entities for mapping success] info = [[iEMS], 12321])</t>
-  </si>
-  <si>
     <t>runid='20211202140114_1_41b809d6-5335-11ec-8833-0242ac12000f'</t>
   </si>
   <si>
@@ -646,6 +643,9 @@
   </si>
   <si>
     <t>motor_current_percent='92.0' and updateTime&lt;'2025-05-21T14:22:43' and id='10100'</t>
+  </si>
+  <si>
+    <t>This entity 12321 is not found in domain [iEMS]</t>
   </si>
 </sst>
 </file>
@@ -1006,8 +1006,8 @@
   <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C84" sqref="C84"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.69140625" defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -1151,10 +1151,10 @@
       <c r="J5" s="3"/>
       <c r="K5" s="4"/>
       <c r="L5" s="3">
-        <v>106920</v>
+        <v>108002</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -2626,7 +2626,7 @@
         <v>142</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -2684,7 +2684,7 @@
         <v>142</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -2858,7 +2858,7 @@
         <v>142</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -3032,7 +3032,7 @@
         <v>142</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -3090,7 +3090,7 @@
         <v>142</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -3119,7 +3119,7 @@
         <v>142</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -3148,7 +3148,7 @@
         <v>142</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -3177,7 +3177,7 @@
         <v>142</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -3206,7 +3206,7 @@
         <v>142</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -3235,7 +3235,7 @@
         <v>142</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
@@ -3264,7 +3264,7 @@
         <v>142</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -3293,7 +3293,7 @@
         <v>142</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -3322,7 +3322,7 @@
         <v>142</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -3351,7 +3351,7 @@
         <v>142</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
@@ -3409,7 +3409,7 @@
         <v>142</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -3438,7 +3438,7 @@
         <v>142</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -3467,7 +3467,7 @@
         <v>142</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
@@ -3496,7 +3496,7 @@
         <v>142</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
@@ -3525,7 +3525,7 @@
         <v>142</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
@@ -3699,7 +3699,7 @@
         <v>142</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
@@ -3757,7 +3757,7 @@
         <v>142</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>

</xml_diff>

<commit_message>
update the test cases for iems
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C037FAC-0BAD-4CB5-A657-1CCC20E7E7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9ED404-E71B-4F8C-88F5-F2D1F263C9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -267,9 +267,6 @@
     <t>id='47'</t>
   </si>
   <si>
-    <t>runid='20220227170207_2_f0d1366c-97ab-11ec-8dcf-0242ac120005'</t>
-  </si>
-  <si>
     <t>iems-connector-test-3-var2</t>
   </si>
   <si>
@@ -316,6 +313,9 @@
   </si>
   <si>
     <t>isTraining=1</t>
+  </si>
+  <si>
+    <t>runid='20230209101323_2_545a4f6e-a81f-11ed-a352-0242ac120005'</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -807,7 +807,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -855,7 +855,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
@@ -1063,7 +1063,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>5</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>5</v>
@@ -1194,7 +1194,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>47</v>
@@ -1246,7 +1246,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
@@ -1298,7 +1298,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>5</v>
@@ -1352,7 +1352,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1454,7 +1454,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1479,13 +1479,13 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>72</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1508,7 +1508,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>72</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>72</v>
@@ -1775,7 +1775,7 @@
         <v>73</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -1804,7 +1804,7 @@
         <v>73</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>

</xml_diff>

<commit_message>
update test cases for iems-test
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iems-connector-test-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codes\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A24D66C-1645-4574-8278-FFC8675CE282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BDD7BD-0C94-4E86-A541-3C73846E1CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="95">
   <si>
     <t>name</t>
   </si>
@@ -216,9 +216,6 @@
     <t>iems-connector-test-mysql-int-3</t>
   </si>
   <si>
-    <t>iems-connector-test-mysql-int-4</t>
-  </si>
-  <si>
     <t>CIMSOURCE_PREDICTRESULT</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
   </si>
   <si>
     <t>idV='47'</t>
-  </si>
-  <si>
-    <t>idV='46'</t>
   </si>
 </sst>
 </file>
@@ -672,11 +666,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K37" sqref="K37"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -807,7 +801,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -855,7 +849,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>5</v>
@@ -953,7 +947,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>5</v>
@@ -1063,7 +1057,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>5</v>
@@ -1113,7 +1107,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>5</v>
@@ -1194,7 +1188,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>47</v>
@@ -1246,7 +1240,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>5</v>
@@ -1298,7 +1292,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>5</v>
@@ -1352,7 +1346,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>5</v>
@@ -1404,7 +1398,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1454,7 +1448,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>5</v>
@@ -1479,13 +1473,13 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1508,13 +1502,13 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -1537,13 +1531,13 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -1569,7 +1563,7 @@
         <v>56</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>58</v>
@@ -1598,7 +1592,7 @@
         <v>57</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>59</v>
@@ -1627,15 +1621,15 @@
         <v>60</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3">
@@ -1656,10 +1650,10 @@
         <v>61</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -1671,11 +1665,9 @@
         <v>0</v>
       </c>
       <c r="I37" s="3">
-        <v>0</v>
-      </c>
-      <c r="J37" s="3">
-        <v>300</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3">
         <v>0</v>
@@ -1687,7 +1679,7 @@
         <v>62</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>65</v>
@@ -1695,14 +1687,14 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3">
         <v>0</v>
       </c>
       <c r="I38" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
@@ -1713,25 +1705,25 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
@@ -1748,19 +1740,19 @@
         <v>72</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
@@ -1771,10 +1763,10 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>92</v>
@@ -1782,7 +1774,7 @@
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3">
@@ -1797,35 +1789,6 @@
         <v>0</v>
       </c>
       <c r="M41" s="3"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3">
-        <v>0</v>
-      </c>
-      <c r="I42" s="3">
-        <v>0</v>
-      </c>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3">
-        <v>0</v>
-      </c>
-      <c r="M42" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>